<commit_message>
Refonte des niveaux pour l'adaptation du procédural, 2 niveaux finis
</commit_message>
<xml_diff>
--- a/Ennemis.xlsx
+++ b/Ennemis.xlsx
@@ -236,9 +236,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -248,6 +245,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -885,10 +885,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:P10"/>
+  <dimension ref="A2:Q10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A10"/>
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -904,7 +904,7 @@
     <col min="14" max="14" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:16" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -944,12 +944,12 @@
       <c r="N2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="O2" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="P2" s="5"/>
+      <c r="P2" s="10"/>
     </row>
-    <row r="3" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -990,10 +990,13 @@
         <v>1</v>
       </c>
       <c r="N3" s="3"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="9"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="8"/>
+      <c r="Q3">
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" spans="1:16" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -1034,10 +1037,13 @@
         <v>1</v>
       </c>
       <c r="N4" s="3"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="8"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="7"/>
+      <c r="Q4">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:16" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -1079,9 +1085,12 @@
       </c>
       <c r="N5" s="3"/>
       <c r="O5" s="2"/>
-      <c r="P5" s="8"/>
+      <c r="P5" s="7"/>
+      <c r="Q5">
+        <v>2</v>
+      </c>
     </row>
-    <row r="6" spans="1:16" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -1122,9 +1131,12 @@
         <v>1.5</v>
       </c>
       <c r="N6" s="3"/>
-      <c r="O6" s="7"/>
+      <c r="O6" s="6"/>
+      <c r="Q6">
+        <v>3</v>
+      </c>
     </row>
-    <row r="7" spans="1:16" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -1165,10 +1177,13 @@
         <v>3</v>
       </c>
       <c r="N7" s="3"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="8"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="7"/>
+      <c r="Q7">
+        <v>1</v>
+      </c>
     </row>
-    <row r="8" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -1210,9 +1225,12 @@
       </c>
       <c r="N8" s="3"/>
       <c r="O8" s="2"/>
-      <c r="P8" s="8"/>
+      <c r="P8" s="7"/>
+      <c r="Q8">
+        <v>4</v>
+      </c>
     </row>
-    <row r="9" spans="1:16" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="69" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -1254,9 +1272,12 @@
       </c>
       <c r="N9" s="3"/>
       <c r="O9" s="2"/>
-      <c r="P9" s="8"/>
+      <c r="P9" s="7"/>
+      <c r="Q9">
+        <v>4</v>
+      </c>
     </row>
-    <row r="10" spans="1:16" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -1297,8 +1318,11 @@
         <v>0.5</v>
       </c>
       <c r="N10" s="3"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="10"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="9"/>
+      <c r="Q10">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>